<commit_message>
pagina quem somos conclída
</commit_message>
<xml_diff>
--- a/Documentação/Timeline/Timeline.xlsx
+++ b/Documentação/Timeline/Timeline.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valemobibr-my.sharepoint.com/personal/vinicius_cano_valemobi_com_br/Documents/Documentos/ads3/grupoPi3Semestre/Documentação/Timeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valemobibr-my.sharepoint.com/personal/vinicius_cano_valemobi_com_br/Documents/Área de Trabalho/SprintBandtec/grupoPi3Semestre/Documentação/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{B2627DEC-2420-4A68-82D5-7A90E95BA1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B327601-0D9F-4BB8-85FD-09974DF9BB13}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{B2627DEC-2420-4A68-82D5-7A90E95BA1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E4D7930-D1DE-46AE-95CA-DD43F887C2F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9FB57336-F48C-432F-BF6B-673F4CBCC94A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9FB57336-F48C-432F-BF6B-673F4CBCC94A}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Título</t>
   </si>
@@ -70,10 +70,13 @@
     <t>BackEnd</t>
   </si>
   <si>
-    <t>FrontEnd</t>
+    <t>Diagrama de Solução de Software</t>
   </si>
   <si>
-    <t>Diagrama de Solução de Software</t>
+    <t>Sprint Backlog</t>
+  </si>
+  <si>
+    <t>FrontEnd</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +174,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -540,11 +549,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -596,33 +699,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
@@ -633,6 +709,66 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018279B4-2725-472F-8F92-8E86BD9C1503}">
   <dimension ref="B1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,67 +1098,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
     </row>
     <row r="2" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="36" t="s">
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="38"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="54"/>
     </row>
     <row r="3" spans="2:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="43"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="15">
         <v>16</v>
       </c>
@@ -1134,7 +1270,7 @@
     </row>
     <row r="4" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="25"/>
@@ -1142,15 +1278,15 @@
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="26"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="45"/>
       <c r="R4" s="27"/>
       <c r="S4" s="13"/>
       <c r="T4" s="8"/>
@@ -1179,19 +1315,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="29"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="46"/>
       <c r="Q5" s="29"/>
       <c r="R5" s="30"/>
       <c r="S5" s="14"/>
@@ -1233,7 +1369,7 @@
       <c r="M6" s="29"/>
       <c r="N6" s="29"/>
       <c r="O6" s="29"/>
-      <c r="P6" s="53"/>
+      <c r="P6" s="42"/>
       <c r="Q6" s="29"/>
       <c r="R6" s="30"/>
       <c r="S6" s="14"/>
@@ -1259,7 +1395,9 @@
       <c r="AM6" s="10"/>
     </row>
     <row r="7" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="28"/>
       <c r="E7" s="29"/>
@@ -1273,17 +1411,17 @@
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
       <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="30"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="38"/>
+      <c r="Z7" s="46"/>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
       <c r="AC7" s="7"/>
@@ -1300,7 +1438,7 @@
     </row>
     <row r="8" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="28"/>
@@ -1310,31 +1448,31 @@
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="30"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="29"/>
-      <c r="W8" s="29"/>
-      <c r="X8" s="29"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
-      <c r="AG8" s="7"/>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="38"/>
+      <c r="Y8" s="38"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="38"/>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="38"/>
+      <c r="AF8" s="38"/>
+      <c r="AG8" s="41"/>
+      <c r="AH8" s="41"/>
+      <c r="AI8" s="46"/>
       <c r="AJ8" s="7"/>
       <c r="AK8" s="7"/>
       <c r="AL8" s="7"/>
@@ -1350,33 +1488,33 @@
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-      <c r="AB9" s="11"/>
-      <c r="AC9" s="11"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="11"/>
-      <c r="AG9" s="11"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="33"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="33"/>
+      <c r="AA9" s="33"/>
+      <c r="AB9" s="33"/>
+      <c r="AC9" s="33"/>
+      <c r="AD9" s="33"/>
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
+      <c r="AG9" s="51"/>
+      <c r="AH9" s="51"/>
+      <c r="AI9" s="47"/>
       <c r="AJ9" s="11"/>
       <c r="AK9" s="11"/>
       <c r="AL9" s="11"/>
@@ -1414,15 +1552,431 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E14CFC-9128-45CB-9376-536E16953BDE}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E1B4BF-A5A6-4A52-B248-0EB1926BD7E1}">
+  <dimension ref="A1:AL9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10:AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="38" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="65"/>
+      <c r="AI2" s="65"/>
+      <c r="AJ2" s="65"/>
+      <c r="AK2" s="65"/>
+      <c r="AL2" s="66"/>
+    </row>
+    <row r="3" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="56"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="72">
+        <v>21</v>
+      </c>
+      <c r="D3" s="72">
+        <v>22</v>
+      </c>
+      <c r="E3" s="72">
+        <v>23</v>
+      </c>
+      <c r="F3" s="72">
+        <v>24</v>
+      </c>
+      <c r="G3" s="72">
+        <v>25</v>
+      </c>
+      <c r="H3" s="72">
+        <v>26</v>
+      </c>
+      <c r="I3" s="72">
+        <v>27</v>
+      </c>
+      <c r="J3" s="72">
+        <v>28</v>
+      </c>
+      <c r="K3" s="72">
+        <v>29</v>
+      </c>
+      <c r="L3" s="72">
+        <v>30</v>
+      </c>
+      <c r="M3" s="72">
+        <v>31</v>
+      </c>
+      <c r="N3" s="72">
+        <v>1</v>
+      </c>
+      <c r="O3" s="72">
+        <v>2</v>
+      </c>
+      <c r="P3" s="72">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="72">
+        <v>4</v>
+      </c>
+      <c r="R3" s="72">
+        <v>5</v>
+      </c>
+      <c r="S3" s="72">
+        <v>6</v>
+      </c>
+      <c r="T3" s="72">
+        <v>7</v>
+      </c>
+      <c r="U3" s="72">
+        <v>8</v>
+      </c>
+      <c r="V3" s="72">
+        <v>9</v>
+      </c>
+      <c r="W3" s="72">
+        <v>10</v>
+      </c>
+      <c r="X3" s="72">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="72">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="72">
+        <v>13</v>
+      </c>
+      <c r="AA3" s="72">
+        <v>14</v>
+      </c>
+      <c r="AB3" s="72">
+        <v>15</v>
+      </c>
+      <c r="AC3" s="72">
+        <v>16</v>
+      </c>
+      <c r="AD3" s="72">
+        <v>17</v>
+      </c>
+      <c r="AE3" s="72">
+        <v>18</v>
+      </c>
+      <c r="AF3" s="72">
+        <v>19</v>
+      </c>
+      <c r="AG3" s="72">
+        <v>20</v>
+      </c>
+      <c r="AH3" s="72">
+        <v>21</v>
+      </c>
+      <c r="AI3" s="72">
+        <v>22</v>
+      </c>
+      <c r="AJ3" s="72">
+        <v>23</v>
+      </c>
+      <c r="AK3" s="72">
+        <v>24</v>
+      </c>
+      <c r="AL3" s="72">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+      <c r="V4" s="68"/>
+      <c r="W4" s="68"/>
+      <c r="X4" s="68"/>
+      <c r="Y4" s="68"/>
+      <c r="Z4" s="68"/>
+      <c r="AA4" s="68"/>
+      <c r="AB4" s="68"/>
+      <c r="AC4" s="68"/>
+      <c r="AD4" s="68"/>
+      <c r="AE4" s="68"/>
+      <c r="AF4" s="68"/>
+      <c r="AG4" s="68"/>
+      <c r="AH4" s="68"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="68"/>
+      <c r="AK4" s="68"/>
+      <c r="AL4" s="70"/>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29"/>
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29"/>
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29"/>
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="30"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="29"/>
+      <c r="Z6" s="29"/>
+      <c r="AA6" s="29"/>
+      <c r="AB6" s="29"/>
+      <c r="AC6" s="29"/>
+      <c r="AD6" s="29"/>
+      <c r="AE6" s="29"/>
+      <c r="AF6" s="29"/>
+      <c r="AG6" s="29"/>
+      <c r="AH6" s="29"/>
+      <c r="AI6" s="29"/>
+      <c r="AJ6" s="29"/>
+      <c r="AK6" s="29"/>
+      <c r="AL6" s="30"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="29"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="29"/>
+      <c r="Z7" s="29"/>
+      <c r="AA7" s="29"/>
+      <c r="AB7" s="29"/>
+      <c r="AC7" s="29"/>
+      <c r="AD7" s="29"/>
+      <c r="AE7" s="29"/>
+      <c r="AF7" s="29"/>
+      <c r="AG7" s="29"/>
+      <c r="AH7" s="29"/>
+      <c r="AI7" s="29"/>
+      <c r="AJ7" s="29"/>
+      <c r="AK7" s="29"/>
+      <c r="AL7" s="30"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="29"/>
+      <c r="Y8" s="29"/>
+      <c r="Z8" s="29"/>
+      <c r="AA8" s="29"/>
+      <c r="AB8" s="29"/>
+      <c r="AC8" s="29"/>
+      <c r="AD8" s="29"/>
+      <c r="AE8" s="29"/>
+      <c r="AF8" s="29"/>
+      <c r="AG8" s="29"/>
+      <c r="AH8" s="29"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
+      <c r="AK8" s="29"/>
+      <c r="AL8" s="30"/>
+    </row>
+    <row r="9" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
+      <c r="AA9" s="32"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
+      <c r="AD9" s="32"/>
+      <c r="AE9" s="32"/>
+      <c r="AF9" s="32"/>
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="32"/>
+      <c r="AI9" s="32"/>
+      <c r="AJ9" s="32"/>
+      <c r="AK9" s="32"/>
+      <c r="AL9" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:Q2"/>
+    <mergeCell ref="R2:AL2"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
white papar, uat e atualizacao docs
</commit_message>
<xml_diff>
--- a/Documentação/Timeline/Timeline.xlsx
+++ b/Documentação/Timeline/Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.cano\OneDrive\OneDrive - VALEMOBI CONSULTORIA EMPRESARIAL S.A\Área de Trabalho\SmartTools\grupoPi3Semestre\Documentação\Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://valemobibr-my.sharepoint.com/personal/vinicius_cano_valemobi_com_br/Documents/Área de Trabalho/Sprint3/grupoPi3Semestre/Documentação/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD5167B-1BAA-4EC3-83A4-9DFE1F810685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{7DD5167B-1BAA-4EC3-83A4-9DFE1F810685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42A3FD8E-9E0C-49BD-9755-40B378877D4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9FB57336-F48C-432F-BF6B-673F4CBCC94A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Título</t>
   </si>
@@ -97,10 +97,13 @@
     <t>Documento de layout</t>
   </si>
   <si>
-    <t>Logs</t>
-  </si>
-  <si>
-    <t>Área Logada FrontEnd</t>
+    <t>Integração telas front</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução de Software - Componentes</t>
+  </si>
+  <si>
+    <t>White Paper</t>
   </si>
 </sst>
 </file>
@@ -147,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="33">
     <border>
@@ -537,19 +546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -589,38 +585,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -629,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -692,72 +705,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,63 +1108,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
     </row>
     <row r="2" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="65" t="s">
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="67"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="79"/>
     </row>
     <row r="3" spans="2:38" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64"/>
+      <c r="B3" s="81"/>
       <c r="C3" s="12">
         <v>16</v>
       </c>
@@ -1528,256 +1550,256 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27E1B4BF-A5A6-4A52-B248-0EB1926BD7E1}">
-  <dimension ref="A1:AT11"/>
+  <dimension ref="A1:AT12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="45" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="79"/>
-      <c r="AC1" s="79"/>
-      <c r="AD1" s="79"/>
-      <c r="AE1" s="79"/>
-      <c r="AF1" s="79"/>
-      <c r="AG1" s="79"/>
-      <c r="AH1" s="79"/>
-      <c r="AI1" s="79"/>
-      <c r="AJ1" s="79"/>
-      <c r="AK1" s="79"/>
-      <c r="AL1" s="79"/>
-      <c r="AM1" s="79"/>
-      <c r="AN1" s="79"/>
-      <c r="AO1" s="79"/>
-      <c r="AP1" s="79"/>
-      <c r="AQ1" s="79"/>
-      <c r="AR1" s="79"/>
-      <c r="AS1" s="79"/>
-      <c r="AT1" s="79"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="66"/>
+      <c r="AO1" s="66"/>
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="66"/>
+      <c r="AS1" s="66"/>
+      <c r="AT1" s="66"/>
     </row>
     <row r="2" spans="1:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="65" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
-      <c r="AC2" s="66"/>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
-      <c r="AF2" s="66"/>
-      <c r="AG2" s="66"/>
-      <c r="AH2" s="66"/>
-      <c r="AI2" s="66"/>
-      <c r="AJ2" s="66"/>
-      <c r="AK2" s="66"/>
-      <c r="AL2" s="66"/>
-      <c r="AM2" s="66"/>
-      <c r="AN2" s="66"/>
-      <c r="AO2" s="66"/>
-      <c r="AP2" s="67"/>
-      <c r="AQ2" s="65" t="s">
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="78"/>
+      <c r="AG2" s="78"/>
+      <c r="AH2" s="78"/>
+      <c r="AI2" s="78"/>
+      <c r="AJ2" s="78"/>
+      <c r="AK2" s="78"/>
+      <c r="AL2" s="78"/>
+      <c r="AM2" s="78"/>
+      <c r="AN2" s="78"/>
+      <c r="AO2" s="78"/>
+      <c r="AP2" s="79"/>
+      <c r="AQ2" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="AR2" s="67"/>
+      <c r="AR2" s="79"/>
     </row>
     <row r="3" spans="1:46" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="72">
+      <c r="A3" s="81"/>
+      <c r="B3" s="59">
         <v>21</v>
       </c>
-      <c r="C3" s="73">
+      <c r="C3" s="60">
         <v>22</v>
       </c>
-      <c r="D3" s="73">
+      <c r="D3" s="60">
         <v>23</v>
       </c>
-      <c r="E3" s="73">
+      <c r="E3" s="60">
         <v>24</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="60">
         <v>25</v>
       </c>
-      <c r="G3" s="73">
+      <c r="G3" s="60">
         <v>26</v>
       </c>
-      <c r="H3" s="73">
+      <c r="H3" s="60">
         <v>27</v>
       </c>
-      <c r="I3" s="73">
+      <c r="I3" s="60">
         <v>28</v>
       </c>
-      <c r="J3" s="73">
+      <c r="J3" s="60">
         <v>29</v>
       </c>
-      <c r="K3" s="73">
+      <c r="K3" s="60">
         <v>30</v>
       </c>
-      <c r="L3" s="74">
+      <c r="L3" s="61">
         <v>31</v>
       </c>
-      <c r="M3" s="72">
+      <c r="M3" s="59">
         <v>1</v>
       </c>
-      <c r="N3" s="73">
+      <c r="N3" s="60">
         <v>2</v>
       </c>
-      <c r="O3" s="73">
+      <c r="O3" s="60">
         <v>3</v>
       </c>
-      <c r="P3" s="73">
+      <c r="P3" s="60">
         <v>4</v>
       </c>
-      <c r="Q3" s="73">
+      <c r="Q3" s="60">
         <v>5</v>
       </c>
-      <c r="R3" s="73">
+      <c r="R3" s="60">
         <v>6</v>
       </c>
-      <c r="S3" s="73">
+      <c r="S3" s="60">
         <v>7</v>
       </c>
-      <c r="T3" s="73">
+      <c r="T3" s="60">
         <v>8</v>
       </c>
-      <c r="U3" s="73">
+      <c r="U3" s="60">
         <v>9</v>
       </c>
-      <c r="V3" s="73">
+      <c r="V3" s="60">
         <v>10</v>
       </c>
-      <c r="W3" s="73">
+      <c r="W3" s="60">
         <v>11</v>
       </c>
-      <c r="X3" s="73">
+      <c r="X3" s="60">
         <v>12</v>
       </c>
-      <c r="Y3" s="73">
+      <c r="Y3" s="60">
         <v>13</v>
       </c>
-      <c r="Z3" s="73">
+      <c r="Z3" s="60">
         <v>14</v>
       </c>
-      <c r="AA3" s="73">
+      <c r="AA3" s="60">
         <v>15</v>
       </c>
-      <c r="AB3" s="73">
+      <c r="AB3" s="60">
         <v>16</v>
       </c>
-      <c r="AC3" s="73">
+      <c r="AC3" s="60">
         <v>17</v>
       </c>
-      <c r="AD3" s="73">
+      <c r="AD3" s="60">
         <v>18</v>
       </c>
-      <c r="AE3" s="73">
+      <c r="AE3" s="60">
         <v>19</v>
       </c>
-      <c r="AF3" s="73">
+      <c r="AF3" s="60">
         <v>20</v>
       </c>
-      <c r="AG3" s="73">
+      <c r="AG3" s="60">
         <v>21</v>
       </c>
-      <c r="AH3" s="73">
+      <c r="AH3" s="60">
         <v>22</v>
       </c>
-      <c r="AI3" s="73">
+      <c r="AI3" s="60">
         <v>23</v>
       </c>
-      <c r="AJ3" s="73">
+      <c r="AJ3" s="60">
         <v>24</v>
       </c>
-      <c r="AK3" s="73">
+      <c r="AK3" s="60">
         <v>25</v>
       </c>
-      <c r="AL3" s="75">
+      <c r="AL3" s="62">
         <v>26</v>
       </c>
-      <c r="AM3" s="75">
+      <c r="AM3" s="62">
         <v>27</v>
       </c>
-      <c r="AN3" s="75">
+      <c r="AN3" s="62">
         <v>28</v>
       </c>
-      <c r="AO3" s="75">
+      <c r="AO3" s="62">
         <v>29</v>
       </c>
-      <c r="AP3" s="76">
+      <c r="AP3" s="63">
         <v>30</v>
       </c>
-      <c r="AQ3" s="77">
+      <c r="AQ3" s="64">
         <v>1</v>
       </c>
-      <c r="AR3" s="78">
+      <c r="AR3" s="65">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
-        <v>20</v>
+      <c r="A4" s="84" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="35"/>
@@ -1790,41 +1812,41 @@
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
       <c r="L4" s="40"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="50"/>
-      <c r="W4" s="50"/>
-      <c r="X4" s="50"/>
-      <c r="Y4" s="50"/>
-      <c r="Z4" s="50"/>
-      <c r="AA4" s="50"/>
-      <c r="AB4" s="50"/>
-      <c r="AC4" s="50"/>
-      <c r="AD4" s="50"/>
-      <c r="AE4" s="50"/>
-      <c r="AF4" s="50"/>
-      <c r="AG4" s="50"/>
-      <c r="AH4" s="50"/>
-      <c r="AI4" s="50"/>
-      <c r="AJ4" s="50"/>
-      <c r="AK4" s="50"/>
-      <c r="AL4" s="50"/>
-      <c r="AM4" s="50"/>
-      <c r="AN4" s="50"/>
-      <c r="AO4" s="50"/>
-      <c r="AP4" s="51"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="42"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="24"/>
       <c r="AQ4" s="22"/>
       <c r="AR4" s="24"/>
     </row>
     <row r="5" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="34"/>
@@ -1838,7 +1860,7 @@
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
       <c r="L5" s="40"/>
-      <c r="M5" s="41"/>
+      <c r="M5" s="34"/>
       <c r="N5" s="35"/>
       <c r="O5" s="35"/>
       <c r="P5" s="35"/>
@@ -1854,12 +1876,12 @@
       <c r="Z5" s="38"/>
       <c r="AA5" s="38"/>
       <c r="AB5" s="43"/>
-      <c r="AC5" s="62"/>
-      <c r="AD5" s="62"/>
-      <c r="AE5" s="62"/>
-      <c r="AF5" s="62"/>
-      <c r="AG5" s="62"/>
-      <c r="AH5" s="62"/>
+      <c r="AC5" s="55"/>
+      <c r="AD5" s="55"/>
+      <c r="AE5" s="55"/>
+      <c r="AF5" s="55"/>
+      <c r="AG5" s="55"/>
+      <c r="AH5" s="55"/>
       <c r="AI5" s="26"/>
       <c r="AJ5" s="26"/>
       <c r="AK5" s="26"/>
@@ -1867,12 +1889,12 @@
       <c r="AM5" s="26"/>
       <c r="AN5" s="26"/>
       <c r="AO5" s="26"/>
-      <c r="AP5" s="52"/>
+      <c r="AP5" s="27"/>
       <c r="AQ5" s="25"/>
       <c r="AR5" s="27"/>
     </row>
     <row r="6" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="56" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="34"/>
@@ -1886,7 +1908,7 @@
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
       <c r="L6" s="40"/>
-      <c r="M6" s="41"/>
+      <c r="M6" s="34"/>
       <c r="N6" s="35"/>
       <c r="O6" s="35"/>
       <c r="P6" s="35"/>
@@ -1915,12 +1937,12 @@
       <c r="AM6" s="26"/>
       <c r="AN6" s="26"/>
       <c r="AO6" s="26"/>
-      <c r="AP6" s="52"/>
+      <c r="AP6" s="27"/>
       <c r="AQ6" s="25"/>
       <c r="AR6" s="27"/>
     </row>
     <row r="7" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="57" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="34"/>
@@ -1931,26 +1953,26 @@
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
       <c r="I7" s="35"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="26"/>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="35"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="38"/>
+      <c r="V7" s="38"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="35"/>
       <c r="AD7" s="26"/>
       <c r="AE7" s="26"/>
       <c r="AF7" s="26"/>
@@ -1963,148 +1985,196 @@
       <c r="AM7" s="26"/>
       <c r="AN7" s="26"/>
       <c r="AO7" s="26"/>
-      <c r="AP7" s="52"/>
+      <c r="AP7" s="27"/>
       <c r="AQ7" s="25"/>
       <c r="AR7" s="27"/>
     </row>
     <row r="8" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="35"/>
-      <c r="AI8" s="38"/>
-      <c r="AJ8" s="38"/>
-      <c r="AK8" s="38"/>
-      <c r="AL8" s="43"/>
-      <c r="AM8" s="26"/>
-      <c r="AN8" s="26"/>
-      <c r="AO8" s="26"/>
-      <c r="AP8" s="52"/>
-      <c r="AQ8" s="25"/>
-      <c r="AR8" s="27"/>
+      <c r="A8" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="68"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
+      <c r="T8" s="69"/>
+      <c r="U8" s="69"/>
+      <c r="V8" s="69"/>
+      <c r="W8" s="69"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="69"/>
+      <c r="Z8" s="85"/>
+      <c r="AA8" s="85"/>
+      <c r="AB8" s="85"/>
+      <c r="AC8" s="86"/>
+      <c r="AD8" s="26"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="26"/>
+      <c r="AI8" s="26"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="26"/>
+      <c r="AL8" s="26"/>
+      <c r="AM8" s="72"/>
+      <c r="AN8" s="72"/>
+      <c r="AO8" s="72"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="73"/>
+      <c r="AR8" s="74"/>
     </row>
-    <row r="9" spans="1:46" ht="27.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71" t="s">
+    <row r="9" spans="1:46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="68"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+      <c r="R9" s="69"/>
+      <c r="S9" s="69"/>
+      <c r="T9" s="69"/>
+      <c r="U9" s="69"/>
+      <c r="V9" s="69"/>
+      <c r="W9" s="71"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="69"/>
+      <c r="Z9" s="69"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="26"/>
+      <c r="AJ9" s="26"/>
+      <c r="AK9" s="26"/>
+      <c r="AL9" s="26"/>
+      <c r="AM9" s="72"/>
+      <c r="AN9" s="72"/>
+      <c r="AO9" s="72"/>
+      <c r="AP9" s="74"/>
+      <c r="AQ9" s="73"/>
+      <c r="AR9" s="74"/>
+    </row>
+    <row r="10" spans="1:46" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="30"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="30"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="30"/>
-      <c r="AG9" s="30"/>
-      <c r="AH9" s="30"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="44"/>
-      <c r="AM9" s="29"/>
-      <c r="AN9" s="29"/>
-      <c r="AO9" s="29"/>
-      <c r="AP9" s="53"/>
-      <c r="AQ9" s="28"/>
-      <c r="AR9" s="49"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="30"/>
+      <c r="V10" s="30"/>
+      <c r="W10" s="67"/>
+      <c r="X10" s="30"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="48"/>
+      <c r="AB10" s="48"/>
+      <c r="AC10" s="48"/>
+      <c r="AD10" s="44"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="29"/>
+      <c r="AG10" s="29"/>
+      <c r="AH10" s="29"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="29"/>
+      <c r="AK10" s="29"/>
+      <c r="AL10" s="29"/>
+      <c r="AM10" s="29"/>
+      <c r="AN10" s="29"/>
+      <c r="AO10" s="29"/>
+      <c r="AP10" s="49"/>
+      <c r="AQ10" s="28"/>
+      <c r="AR10" s="49"/>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B11" s="61" t="s">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="B12" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="54" t="s">
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="54" t="s">
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="54" t="s">
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="52"/>
+      <c r="V12" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="W11" s="54"/>
-      <c r="X11" s="54"/>
-      <c r="Y11" s="54"/>
-      <c r="Z11" s="54"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="54" t="s">
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="53"/>
+      <c r="AC12" s="50" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="M2:AP2"/>
     <mergeCell ref="AQ2:AR2"/>

</xml_diff>